<commit_message>
NAV-38 format test data sheet
</commit_message>
<xml_diff>
--- a/Estimates_Navigator_BDG_Validations.xlsx
+++ b/Estimates_Navigator_BDG_Validations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jyri\ubuntu_projects\navigator\navigator_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E830A3F8-13C9-4B2A-AC76-D56A1494D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA682D2-6589-40C9-A260-F755B4C576BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="1140" windowWidth="20052" windowHeight="9720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="972" yWindow="1020" windowWidth="20052" windowHeight="10620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="320">
   <si>
     <t>What is this file?</t>
   </si>
@@ -927,9 +927,6 @@
     <t>Populate Shiny 90 HIV testing template</t>
   </si>
   <si>
-    <t>Resources</t>
-  </si>
-  <si>
     <t>Does user have an ADR user account?</t>
   </si>
   <si>
@@ -1284,23 +1281,38 @@
     <t>Entry Criteria</t>
   </si>
   <si>
-    <t>Skippable</t>
-  </si>
-  <si>
     <t>General estimates data from HMIS</t>
   </si>
   <si>
-    <t>If test fails, skip to the following row:</t>
-  </si>
-  <si>
     <t>If test fails, skip to this row:</t>
+  </si>
+  <si>
+    <t>02-1</t>
+  </si>
+  <si>
+    <t>02-2</t>
+  </si>
+  <si>
+    <t>02-3</t>
+  </si>
+  <si>
+    <t>02-4</t>
+  </si>
+  <si>
+    <t>02-5</t>
+  </si>
+  <si>
+    <t>02-6</t>
+  </si>
+  <si>
+    <t>02-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1421,13 +1433,6 @@
     </font>
     <font>
       <strike/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1478,7 +1483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1572,21 +1577,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -1663,15 +1653,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1730,7 +1711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1787,13 +1768,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1843,10 +1818,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1861,7 +1833,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1869,22 +1841,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1893,31 +1862,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2173,8 +2136,8 @@
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>290</v>
+      <c r="A5" s="45" t="s">
+        <v>289</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -2186,7 +2149,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8417,8 +8380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J997"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8435,45 +8398,45 @@
     <col min="10" max="26" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="63" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
-        <v>305</v>
-      </c>
-      <c r="B1" s="79" t="s">
+    <row r="1" spans="1:10" s="60" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="72" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>310</v>
+      </c>
+      <c r="E1" s="77"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+    </row>
+    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="79" t="s">
-        <v>310</v>
-      </c>
-      <c r="D1" s="81" t="s">
-        <v>311</v>
-      </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-    </row>
-    <row r="2" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62" t="s">
-        <v>313</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>308</v>
-      </c>
-      <c r="C2" s="62" t="s">
-        <v>310</v>
-      </c>
-      <c r="D2" s="80" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="75"/>
+      <c r="C2" s="59" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" s="74" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="78"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
@@ -8495,11 +8458,11 @@
       <c r="C4" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="E4" s="77" t="s">
-        <v>315</v>
+      <c r="E4" s="71" t="s">
+        <v>312</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>8</v>
@@ -8513,8 +8476,8 @@
       <c r="I4" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="J4" s="49" t="s">
-        <v>278</v>
+      <c r="J4" s="47" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="112.8" x14ac:dyDescent="0.25">
@@ -8524,11 +8487,11 @@
       <c r="B5" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="46" t="s">
         <v>276</v>
-      </c>
-      <c r="D5" s="48" t="s">
-        <v>277</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="16">
@@ -8537,11 +8500,11 @@
       <c r="G5" s="17">
         <v>0</v>
       </c>
-      <c r="H5" s="48" t="s">
-        <v>291</v>
+      <c r="H5" s="46" t="s">
+        <v>290</v>
       </c>
       <c r="I5" s="18"/>
-      <c r="J5" s="27"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" spans="1:10" ht="102.6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -8561,16 +8524,16 @@
       <c r="G6" s="20"/>
       <c r="H6" s="21"/>
       <c r="I6" s="20"/>
-      <c r="J6" s="48"/>
+      <c r="J6" s="46"/>
     </row>
     <row r="7" spans="1:10" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B7" s="58" t="s">
-        <v>293</v>
-      </c>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="55" t="s">
+        <v>292</v>
+      </c>
+      <c r="C7" s="56" t="s">
         <v>203</v>
       </c>
       <c r="D7" s="22"/>
@@ -8584,12 +8547,12 @@
         <v>0</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>294</v>
-      </c>
-      <c r="I7" s="55" t="s">
+        <v>293</v>
+      </c>
+      <c r="I7" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="50"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" spans="1:10" ht="163.80000000000001" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
@@ -8612,10 +8575,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="I8" s="55"/>
-      <c r="J8" s="50"/>
+        <v>294</v>
+      </c>
+      <c r="I8" s="52"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" spans="1:10" ht="245.4" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -8637,20 +8600,20 @@
       <c r="G9" s="17">
         <v>1</v>
       </c>
-      <c r="H9" s="50" t="s">
-        <v>292</v>
-      </c>
-      <c r="I9" s="55"/>
+      <c r="H9" s="48" t="s">
+        <v>291</v>
+      </c>
+      <c r="I9" s="52"/>
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>214</v>
       </c>
       <c r="D10" s="25"/>
@@ -8662,21 +8625,21 @@
         <v>1</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>279</v>
-      </c>
-      <c r="I10" s="55"/>
+        <v>278</v>
+      </c>
+      <c r="I10" s="52"/>
       <c r="J10" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="153.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="46" t="s">
         <v>217</v>
       </c>
       <c r="D11" s="25"/>
@@ -8687,22 +8650,22 @@
       <c r="G11" s="17">
         <v>1</v>
       </c>
-      <c r="H11" s="50" t="s">
-        <v>280</v>
-      </c>
-      <c r="I11" s="55"/>
+      <c r="H11" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="I11" s="52"/>
       <c r="J11" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="174" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>220</v>
       </c>
       <c r="D12" s="25"/>
@@ -8713,19 +8676,19 @@
       <c r="G12" s="17">
         <v>1</v>
       </c>
-      <c r="H12" s="50" t="s">
-        <v>280</v>
-      </c>
-      <c r="I12" s="55"/>
+      <c r="H12" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="I12" s="52"/>
       <c r="J12" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
+      <c r="B14" s="57"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9969,8 +9932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9982,107 +9945,107 @@
     <col min="5" max="5" width="23.69921875" customWidth="1"/>
     <col min="6" max="6" width="11.8984375" customWidth="1"/>
     <col min="7" max="7" width="30.69921875" customWidth="1"/>
-    <col min="8" max="8" width="30.69921875" style="57" customWidth="1"/>
+    <col min="8" max="8" width="30.69921875" style="54" customWidth="1"/>
     <col min="9" max="9" width="33.19921875" customWidth="1"/>
     <col min="10" max="10" width="22.09765625" customWidth="1"/>
     <col min="11" max="27" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="65" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>310</v>
+      </c>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+    </row>
+    <row r="2" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="67" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B2" s="68" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="69" t="s">
-        <v>310</v>
-      </c>
-      <c r="D1" s="71" t="s">
-        <v>311</v>
-      </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-    </row>
-    <row r="2" spans="1:11" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
-        <v>306</v>
-      </c>
-      <c r="B2" s="73" t="s">
+      <c r="C2" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="73" t="s">
-        <v>309</v>
-      </c>
-      <c r="D2" s="74" t="s">
-        <v>281</v>
-      </c>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-    </row>
-    <row r="3" spans="1:11" s="57" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
+      <c r="D2" s="69" t="s">
+        <v>280</v>
+      </c>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="79" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>312</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="J4" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="K4" s="62" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="61.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="64" t="s">
-        <v>314</v>
-      </c>
-      <c r="F4" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="64" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="76" t="s">
-        <v>195</v>
-      </c>
-      <c r="I4" s="77" t="s">
-        <v>312</v>
-      </c>
-      <c r="J4" s="69" t="s">
-        <v>194</v>
-      </c>
-      <c r="K4" s="67" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="61.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
-        <v>1</v>
-      </c>
-      <c r="B5" s="21" t="s">
+      <c r="C5" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="D5" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="23">
         <v>0</v>
       </c>
@@ -10090,28 +10053,28 @@
         <v>0</v>
       </c>
       <c r="H5" s="25"/>
-      <c r="I5" s="27" t="b">
+      <c r="I5" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="48" t="s">
-        <v>282</v>
-      </c>
-      <c r="K5" s="48"/>
-    </row>
-    <row r="6" spans="1:11" ht="72.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
-        <v>2</v>
+      <c r="J5" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="K5" s="46"/>
+    </row>
+    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>314</v>
       </c>
       <c r="B6" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>226</v>
-      </c>
       <c r="D6" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6" s="27"/>
+        <v>223</v>
+      </c>
+      <c r="E6" s="26"/>
       <c r="F6" s="23">
         <v>0</v>
       </c>
@@ -10119,24 +10082,24 @@
         <v>0</v>
       </c>
       <c r="H6" s="25"/>
-      <c r="I6" s="27" t="b">
+      <c r="I6" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-    </row>
-    <row r="7" spans="1:11" ht="93" x14ac:dyDescent="0.3">
-      <c r="A7" s="28">
-        <v>3</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>300</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>228</v>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>227</v>
       </c>
       <c r="D7" s="25"/>
-      <c r="E7" s="27"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="23">
         <v>0</v>
       </c>
@@ -10144,28 +10107,28 @@
         <v>1</v>
       </c>
       <c r="H7" s="25"/>
-      <c r="I7" s="27" t="b">
+      <c r="I7" s="26" t="b">
         <v>0</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="K7" s="50" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="286.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="52">
-        <v>4</v>
-      </c>
-      <c r="B8" s="53" t="s">
-        <v>286</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>227</v>
+        <v>298</v>
+      </c>
+      <c r="K7" s="48" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="286.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="D8" s="25"/>
-      <c r="E8" s="27"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="23">
         <v>0</v>
       </c>
@@ -10173,30 +10136,30 @@
         <v>1</v>
       </c>
       <c r="H8" s="25"/>
-      <c r="I8" s="27" t="b">
+      <c r="I8" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="46" t="s">
+        <v>287</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="46" t="s">
         <v>288</v>
       </c>
-      <c r="K8" s="48" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="93" x14ac:dyDescent="0.3">
-      <c r="A9" s="28">
-        <v>5</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>302</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>289</v>
-      </c>
-      <c r="E9" s="48"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="23">
         <v>1</v>
       </c>
@@ -10204,55 +10167,55 @@
         <v>1</v>
       </c>
       <c r="H9" s="25"/>
-      <c r="I9" s="27" t="b">
+      <c r="I9" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="J9" s="27" t="s">
-        <v>301</v>
-      </c>
-      <c r="K9" s="27"/>
-    </row>
-    <row r="10" spans="1:11" s="56" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="28">
-        <v>6</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>303</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
+      <c r="J9" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="1:11" s="53" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27" t="b">
+      <c r="H10" s="26"/>
+      <c r="I10" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="1:11" ht="72.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A11" s="28">
-        <v>7</v>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>319</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="27"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="25"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
-      <c r="I11" s="27" t="b">
+      <c r="I11" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="J11" s="48" t="s">
-        <v>287</v>
-      </c>
-      <c r="K11" s="27"/>
+      <c r="J11" s="46" t="s">
+        <v>286</v>
+      </c>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="6"/>
@@ -10641,334 +10604,334 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="31" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35" t="s">
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="37" t="s">
+      <c r="H3" s="36"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="H3" s="38"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="39" t="s">
+      <c r="H4" s="38"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="H4" s="40"/>
-    </row>
-    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="37" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="39" t="s">
+      <c r="H5" s="38"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="41" t="s">
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="H6" s="42"/>
-    </row>
-    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="39" t="s">
+      <c r="H7" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="H7" s="43" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+      <c r="B8" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="37" t="s">
         <v>248</v>
       </c>
-      <c r="B8" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="39" t="s">
+      <c r="H8" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="H8" s="43" t="s">
+    </row>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35" t="s">
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="H9" s="36"/>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="37" t="s">
+      <c r="H10" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="H10" s="29" t="s">
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="42" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="44" t="s">
+      <c r="H11" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="H11" s="29" t="s">
+    </row>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="37" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="39" t="s">
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="H12" s="29"/>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="44" t="s">
+      <c r="H13" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="H13" s="29" t="s">
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35" t="s">
+      <c r="H14" s="34"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="H14" s="36"/>
-    </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="37" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="43" t="s">
         <v>262</v>
       </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="45" t="s">
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="35" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="37" t="s">
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="H16" s="29"/>
-    </row>
-    <row r="17" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="37" t="s">
+      <c r="H17" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="H17" s="29" t="s">
+    </row>
+    <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="42" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="44" t="s">
+      <c r="H18" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="H18" s="29" t="s">
+    </row>
+    <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35" t="s">
+      <c r="H19" s="34"/>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="42" t="s">
         <v>269</v>
       </c>
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="44" t="s">
+      <c r="H20" s="36"/>
+    </row>
+    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="H20" s="38"/>
-    </row>
-    <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="37" t="s">
+      <c r="H21" s="36"/>
+    </row>
+    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="42" t="s">
         <v>271</v>
       </c>
-      <c r="H21" s="38"/>
-    </row>
-    <row r="22" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="44" t="s">
+      <c r="H22" s="36"/>
+    </row>
+    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="35" t="s">
         <v>272</v>
       </c>
-      <c r="H22" s="38"/>
-    </row>
-    <row r="23" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="37" t="s">
+      <c r="H23" s="36"/>
+    </row>
+    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="44" t="s">
         <v>273</v>
       </c>
-      <c r="H23" s="38"/>
-    </row>
-    <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="46" t="s">
-        <v>274</v>
-      </c>
-      <c r="H24" s="46"/>
+      <c r="H24" s="44"/>
     </row>
     <row r="25" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
NAV-59 Working decision graph source file
</commit_message>
<xml_diff>
--- a/Estimates_Navigator_BDG_Validations.xlsx
+++ b/Estimates_Navigator_BDG_Validations.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="321">
   <si>
     <t xml:space="preserve">Ref.</t>
   </si>
@@ -1164,9 +1164,6 @@
     <t xml:space="preserve"> Data input files are available
  User has an ADR account associated with a country organization in ADR
  User has at least editor role assigned within the country organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action Content</t>
   </si>
   <si>
     <t xml:space="preserve">Check if GeoJSON uploaded</t>
@@ -10103,7 +10100,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10158,7 +10155,7 @@
         <v>193</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>308</v>
+        <v>194</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>195</v>
@@ -10184,16 +10181,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>310</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>311</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
@@ -10201,7 +10198,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J5" s="16"/>
       <c r="K5" s="14"/>
@@ -10211,16 +10208,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C6" s="46" t="s">
         <v>203</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>314</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>315</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -10228,7 +10225,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="14"/>
@@ -10238,16 +10235,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C7" s="46" t="s">
         <v>242</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>317</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>318</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -10255,7 +10252,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J7" s="21"/>
       <c r="K7" s="20"/>
@@ -10265,16 +10262,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C8" s="46" t="s">
         <v>203</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>320</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>321</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -10282,7 +10279,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J8" s="18"/>
       <c r="K8" s="14"/>

</xml_diff>

<commit_message>
NAV-75 Graph loading logic for node refs
</commit_message>
<xml_diff>
--- a/Estimates_Navigator_BDG_Validations.xlsx
+++ b/Estimates_Navigator_BDG_Validations.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="325">
   <si>
     <t xml:space="preserve">Ref.</t>
   </si>
@@ -804,7 +804,7 @@
     <t xml:space="preserve">S4 Follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">00-1</t>
+    <t xml:space="preserve">0-0</t>
   </si>
   <si>
     <t xml:space="preserve">Are you ready to run milestone 01?</t>
@@ -819,13 +819,13 @@
     <t xml:space="preserve">These are the things you need to do to run milestone 01.</t>
   </si>
   <si>
-    <t xml:space="preserve">00-2</t>
+    <t xml:space="preserve">0-1</t>
   </si>
   <si>
     <t xml:space="preserve">01-GenEstsDataHMIS</t>
   </si>
   <si>
-    <t xml:space="preserve">00-3</t>
+    <t xml:space="preserve">0-2</t>
   </si>
   <si>
     <t xml:space="preserve">Are you ready to run milestone 02?</t>
@@ -837,7 +837,7 @@
     <t xml:space="preserve">These are the things you need to do to run milestone 02.</t>
   </si>
   <si>
-    <t xml:space="preserve">00-4</t>
+    <t xml:space="preserve">0-3</t>
   </si>
   <si>
     <t xml:space="preserve">02-UploadDataADR</t>
@@ -851,7 +851,7 @@
  The user is authorized to prepare estimates on behalf of the country</t>
   </si>
   <si>
-    <t xml:space="preserve">01-1</t>
+    <t xml:space="preserve">1-0</t>
   </si>
   <si>
     <t xml:space="preserve">Have all programme data required for estimates been completed and are they available in the national health information system?</t>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">MM: Add sheet to HIV tools page and put link to that sheet here</t>
   </si>
   <si>
-    <t xml:space="preserve">01-2</t>
+    <t xml:space="preserve">1-1</t>
   </si>
   <si>
     <t xml:space="preserve">Has the country team conducted data quality procedures on each of the required data inputs using Guide 6, Data Quality Standards of Practice?</t>
@@ -884,19 +884,19 @@
     <t xml:space="preserve">Guide 6, Data Quality Standards of Practice https://hivtools.unaids.org/hiv-estimates-training-material-en/</t>
   </si>
   <si>
-    <t xml:space="preserve">01-3</t>
+    <t xml:space="preserve">1-2</t>
   </si>
   <si>
     <t xml:space="preserve">Will the country produce district estimates?</t>
   </si>
   <si>
-    <t xml:space="preserve">01-5</t>
+    <t xml:space="preserve">1-4</t>
   </si>
   <si>
     <t xml:space="preserve">2023+ as all generalized epi countries use Naomi</t>
   </si>
   <si>
-    <t xml:space="preserve">01-4</t>
+    <t xml:space="preserve">1-3</t>
   </si>
   <si>
     <t xml:space="preserve">Have you downloaded the data input templates from ADR?</t>
@@ -938,16 +938,16 @@
     <t xml:space="preserve">return_false()</t>
   </si>
   <si>
-    <t xml:space="preserve">01-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the user completed skippable action 01-4?</t>
+    <t xml:space="preserve">1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the user completed skippable action 1-3?</t>
   </si>
   <si>
     <t xml:space="preserve">Skip check</t>
   </si>
   <si>
-    <t xml:space="preserve">01-7</t>
+    <t xml:space="preserve">1-6</t>
   </si>
   <si>
     <t xml:space="preserve">Will the country be utilizing Shiny 90 to produce knowledge of status estimates?</t>
@@ -993,7 +993,7 @@
     <t xml:space="preserve">28/oct - MM: although we know most countries who will use s90, we should put the burden on the user to confirm. </t>
   </si>
   <si>
-    <t xml:space="preserve">01-8</t>
+    <t xml:space="preserve">1-7</t>
   </si>
   <si>
     <t xml:space="preserve">Is Shiny 90 survey template populated?</t>
@@ -1008,7 +1008,7 @@
     <t xml:space="preserve">28/oct - instruct user to pull last year's survey file for S90 into this year's inputs package. Download the file and update it with any updated survey data. </t>
   </si>
   <si>
-    <t xml:space="preserve">01-9</t>
+    <t xml:space="preserve">1-8</t>
   </si>
   <si>
     <t xml:space="preserve">Is Shiny 90 HIV Testing template populated?</t>
@@ -1166,6 +1166,9 @@
  User has at least editor role assigned within the country organization</t>
   </si>
   <si>
+    <t xml:space="preserve">2-0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if GeoJSON uploaded</t>
   </si>
   <si>
@@ -1178,6 +1181,9 @@
     <t xml:space="preserve">url</t>
   </si>
   <si>
+    <t xml:space="preserve">2-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if GeoJSON valid</t>
   </si>
   <si>
@@ -1187,6 +1193,9 @@
     <t xml:space="preserve">Validate geographic data html</t>
   </si>
   <si>
+    <t xml:space="preserve">2-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if Survey data uploaded</t>
   </si>
   <si>
@@ -1194,6 +1203,9 @@
   </si>
   <si>
     <t xml:space="preserve">Upload survey data html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3</t>
   </si>
   <si>
     <t xml:space="preserve">Check if Survey data valid</t>
@@ -1275,6 +1287,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1297,6 +1316,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -1310,25 +1335,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <strike val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1506,12 +1518,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1550,27 +1566,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1582,7 +1602,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1590,60 +1610,52 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1729,18 +1741,18 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.2"/>
@@ -6951,11 +6963,11 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.9"/>
@@ -7044,10 +7056,10 @@
         <v>205</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7061,10 +7073,10 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="18"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7083,12 +7095,12 @@
       <c r="E7" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
@@ -7101,10 +7113,10 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="18"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7126,22 +7138,23 @@
   </sheetPr>
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="37.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="63.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="11.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="11" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="12" style="0" width="7.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7157,31 +7170,31 @@
       <c r="D1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -7196,21 +7209,21 @@
       <c r="D2" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
@@ -7248,7 +7261,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>216</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -7263,21 +7276,21 @@
       <c r="E5" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="15" t="n">
+      <c r="F5" s="15"/>
+      <c r="G5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>222</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -7292,44 +7305,44 @@
       <c r="E6" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="17"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="14"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="13" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="G7" s="15" t="n">
+      <c r="G7" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>231</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -7344,21 +7357,21 @@
       <c r="E8" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="15" t="n">
+      <c r="F8" s="15"/>
+      <c r="G8" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="15" t="s">
         <v>229</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -7373,21 +7386,21 @@
       <c r="E9" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="15" t="n">
+      <c r="F9" s="15"/>
+      <c r="G9" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="16" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="17" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="15" t="s">
         <v>243</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -7398,19 +7411,19 @@
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="15" t="n">
+      <c r="F10" s="15"/>
+      <c r="G10" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="16" t="s">
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="15" t="s">
         <v>246</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -7419,25 +7432,25 @@
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="G11" s="15" t="n">
+      <c r="G11" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="20" t="s">
+      <c r="I11" s="22"/>
+      <c r="J11" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="15" t="s">
         <v>251</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -7450,23 +7463,23 @@
         <v>253</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="15" t="n">
+      <c r="F12" s="15"/>
+      <c r="G12" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="22"/>
+      <c r="J12" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="15" t="s">
         <v>256</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -7479,18 +7492,18 @@
         <v>258</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="15" t="n">
+      <c r="F13" s="15"/>
+      <c r="G13" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="17" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7498,9 +7511,9 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8760,11 +8773,11 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.2"/>
@@ -8775,151 +8788,151 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="33" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="H2" s="36"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="37" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="H3" s="38"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="39" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="H4" s="40"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="39" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="41" t="s">
         <v>272</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="41" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="43" t="s">
         <v>274</v>
       </c>
-      <c r="H6" s="42"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="39" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="45" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="B8" s="32" t="n">
+      <c r="B8" s="34" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="39" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="45" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="37" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="39" t="s">
         <v>284</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -8927,13 +8940,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="44" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="46" t="s">
         <v>286</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -8941,25 +8954,25 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="39" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="41" t="s">
         <v>288</v>
       </c>
       <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="44" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="46" t="s">
         <v>289</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -8967,52 +8980,52 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37" t="s">
         <v>291</v>
       </c>
-      <c r="H14" s="36"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="37" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="39" t="s">
         <v>292</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="25" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="37" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="39" t="s">
         <v>294</v>
       </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="37" t="s">
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="39" t="s">
         <v>295</v>
       </c>
       <c r="H17" s="7" t="s">
@@ -9020,13 +9033,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="44" t="s">
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="46" t="s">
         <v>297</v>
       </c>
       <c r="H18" s="7" t="s">
@@ -9034,76 +9047,76 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35" t="s">
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="H19" s="36"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="44" t="s">
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="46" t="s">
         <v>300</v>
       </c>
-      <c r="H20" s="38"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="37" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="39" t="s">
         <v>301</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="44" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="H22" s="38"/>
+      <c r="H22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="37" t="s">
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="39" t="s">
         <v>303</v>
       </c>
-      <c r="H23" s="38"/>
+      <c r="H23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="45" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="47" t="s">
         <v>304</v>
       </c>
-      <c r="H24" s="45"/>
+      <c r="H24" s="47"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10099,11 +10112,11 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.9"/>
@@ -10177,111 +10190,111 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
-        <v>1</v>
+      <c r="A5" s="15" t="s">
+        <v>308</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="E5" s="13" t="s">
         <v>310</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>311</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="15" t="n">
+      <c r="H5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="J5" s="16"/>
+        <v>312</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="K5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
-        <v>2</v>
+      <c r="A6" s="15" t="s">
+        <v>313</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="C6" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>314</v>
+        <v>315</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="17" t="n">
+      <c r="H6" s="18" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="J6" s="18"/>
+        <v>312</v>
+      </c>
+      <c r="J6" s="19"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
-        <v>3</v>
+      <c r="A7" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="C7" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>242</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>317</v>
+        <v>319</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="47" t="n">
+      <c r="H7" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
+      <c r="I7" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
-        <v>4</v>
+      <c r="A8" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C8" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>320</v>
+        <v>323</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>324</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="17" t="n">
+      <c r="H8" s="18" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="J8" s="18"/>
+        <v>312</v>
+      </c>
+      <c r="J8" s="19"/>
       <c r="K8" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nav 75 Introduce node refs (#30)
* NAV-75 Model update to include node refs

* NAV-75 Decision engine and progress tracker updates for refs

* NAV-75 Fix tests

* NAV-75 Graph loading logic for node refs

* NAV-75 Fix end to end test
</commit_message>
<xml_diff>
--- a/Estimates_Navigator_BDG_Validations.xlsx
+++ b/Estimates_Navigator_BDG_Validations.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="325">
   <si>
     <t xml:space="preserve">Ref.</t>
   </si>
@@ -804,7 +804,7 @@
     <t xml:space="preserve">S4 Follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">00-1</t>
+    <t xml:space="preserve">0-0</t>
   </si>
   <si>
     <t xml:space="preserve">Are you ready to run milestone 01?</t>
@@ -819,13 +819,13 @@
     <t xml:space="preserve">These are the things you need to do to run milestone 01.</t>
   </si>
   <si>
-    <t xml:space="preserve">00-2</t>
+    <t xml:space="preserve">0-1</t>
   </si>
   <si>
     <t xml:space="preserve">01-GenEstsDataHMIS</t>
   </si>
   <si>
-    <t xml:space="preserve">00-3</t>
+    <t xml:space="preserve">0-2</t>
   </si>
   <si>
     <t xml:space="preserve">Are you ready to run milestone 02?</t>
@@ -837,7 +837,7 @@
     <t xml:space="preserve">These are the things you need to do to run milestone 02.</t>
   </si>
   <si>
-    <t xml:space="preserve">00-4</t>
+    <t xml:space="preserve">0-3</t>
   </si>
   <si>
     <t xml:space="preserve">02-UploadDataADR</t>
@@ -851,7 +851,7 @@
  The user is authorized to prepare estimates on behalf of the country</t>
   </si>
   <si>
-    <t xml:space="preserve">01-1</t>
+    <t xml:space="preserve">1-0</t>
   </si>
   <si>
     <t xml:space="preserve">Have all programme data required for estimates been completed and are they available in the national health information system?</t>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">MM: Add sheet to HIV tools page and put link to that sheet here</t>
   </si>
   <si>
-    <t xml:space="preserve">01-2</t>
+    <t xml:space="preserve">1-1</t>
   </si>
   <si>
     <t xml:space="preserve">Has the country team conducted data quality procedures on each of the required data inputs using Guide 6, Data Quality Standards of Practice?</t>
@@ -884,19 +884,19 @@
     <t xml:space="preserve">Guide 6, Data Quality Standards of Practice https://hivtools.unaids.org/hiv-estimates-training-material-en/</t>
   </si>
   <si>
-    <t xml:space="preserve">01-3</t>
+    <t xml:space="preserve">1-2</t>
   </si>
   <si>
     <t xml:space="preserve">Will the country produce district estimates?</t>
   </si>
   <si>
-    <t xml:space="preserve">01-5</t>
+    <t xml:space="preserve">1-4</t>
   </si>
   <si>
     <t xml:space="preserve">2023+ as all generalized epi countries use Naomi</t>
   </si>
   <si>
-    <t xml:space="preserve">01-4</t>
+    <t xml:space="preserve">1-3</t>
   </si>
   <si>
     <t xml:space="preserve">Have you downloaded the data input templates from ADR?</t>
@@ -938,16 +938,16 @@
     <t xml:space="preserve">return_false()</t>
   </si>
   <si>
-    <t xml:space="preserve">01-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the user completed skippable action 01-4?</t>
+    <t xml:space="preserve">1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the user completed skippable action 1-3?</t>
   </si>
   <si>
     <t xml:space="preserve">Skip check</t>
   </si>
   <si>
-    <t xml:space="preserve">01-7</t>
+    <t xml:space="preserve">1-6</t>
   </si>
   <si>
     <t xml:space="preserve">Will the country be utilizing Shiny 90 to produce knowledge of status estimates?</t>
@@ -993,7 +993,7 @@
     <t xml:space="preserve">28/oct - MM: although we know most countries who will use s90, we should put the burden on the user to confirm. </t>
   </si>
   <si>
-    <t xml:space="preserve">01-8</t>
+    <t xml:space="preserve">1-7</t>
   </si>
   <si>
     <t xml:space="preserve">Is Shiny 90 survey template populated?</t>
@@ -1008,7 +1008,7 @@
     <t xml:space="preserve">28/oct - instruct user to pull last year's survey file for S90 into this year's inputs package. Download the file and update it with any updated survey data. </t>
   </si>
   <si>
-    <t xml:space="preserve">01-9</t>
+    <t xml:space="preserve">1-8</t>
   </si>
   <si>
     <t xml:space="preserve">Is Shiny 90 HIV Testing template populated?</t>
@@ -1166,6 +1166,9 @@
  User has at least editor role assigned within the country organization</t>
   </si>
   <si>
+    <t xml:space="preserve">2-0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if GeoJSON uploaded</t>
   </si>
   <si>
@@ -1178,6 +1181,9 @@
     <t xml:space="preserve">url</t>
   </si>
   <si>
+    <t xml:space="preserve">2-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if GeoJSON valid</t>
   </si>
   <si>
@@ -1187,6 +1193,9 @@
     <t xml:space="preserve">Validate geographic data html</t>
   </si>
   <si>
+    <t xml:space="preserve">2-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if Survey data uploaded</t>
   </si>
   <si>
@@ -1194,6 +1203,9 @@
   </si>
   <si>
     <t xml:space="preserve">Upload survey data html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3</t>
   </si>
   <si>
     <t xml:space="preserve">Check if Survey data valid</t>
@@ -1275,6 +1287,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1297,6 +1316,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -1310,25 +1335,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <strike val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1506,12 +1518,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1550,27 +1566,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1582,7 +1602,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1590,60 +1610,52 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1729,18 +1741,18 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.2"/>
@@ -6951,11 +6963,11 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.9"/>
@@ -7044,10 +7056,10 @@
         <v>205</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="14"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7061,10 +7073,10 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="14"/>
-      <c r="J6" s="18"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7083,12 +7095,12 @@
       <c r="E7" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
@@ -7101,10 +7113,10 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="18"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7126,22 +7138,23 @@
   </sheetPr>
   <dimension ref="A1:AD1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="37.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="63.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="0" width="11.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="11" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="12" style="0" width="7.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7157,31 +7170,31 @@
       <c r="D1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
     </row>
     <row r="2" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -7196,21 +7209,21 @@
       <c r="D2" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
@@ -7248,7 +7261,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>216</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -7263,21 +7276,21 @@
       <c r="E5" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="15" t="n">
+      <c r="F5" s="15"/>
+      <c r="G5" s="16" t="n">
         <v>1</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>222</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -7292,44 +7305,44 @@
       <c r="E6" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="17"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="14"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="19"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="13" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="G7" s="15" t="n">
+      <c r="G7" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="16" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>231</v>
       </c>
       <c r="B8" s="14" t="s">
@@ -7344,21 +7357,21 @@
       <c r="E8" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="15" t="n">
+      <c r="F8" s="15"/>
+      <c r="G8" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="22"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="57.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="15" t="s">
         <v>229</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -7373,21 +7386,21 @@
       <c r="E9" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="15" t="n">
+      <c r="F9" s="15"/>
+      <c r="G9" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="16" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="17" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="15" t="s">
         <v>243</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -7398,19 +7411,19 @@
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="15" t="n">
+      <c r="F10" s="15"/>
+      <c r="G10" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="16" t="s">
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="15" t="s">
         <v>246</v>
       </c>
       <c r="B11" s="14" t="s">
@@ -7419,25 +7432,25 @@
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="G11" s="15" t="n">
+      <c r="G11" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="20" t="s">
+      <c r="I11" s="22"/>
+      <c r="J11" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="15" t="s">
         <v>251</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -7450,23 +7463,23 @@
         <v>253</v>
       </c>
       <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="15" t="n">
+      <c r="F12" s="15"/>
+      <c r="G12" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="20" t="s">
+      <c r="I12" s="22"/>
+      <c r="J12" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="15" t="s">
         <v>256</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -7479,18 +7492,18 @@
         <v>258</v>
       </c>
       <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="15" t="n">
+      <c r="F13" s="15"/>
+      <c r="G13" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="I13" s="21"/>
-      <c r="J13" s="20" t="s">
+      <c r="I13" s="22"/>
+      <c r="J13" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="17" t="s">
         <v>203</v>
       </c>
     </row>
@@ -7498,9 +7511,9 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8760,11 +8773,11 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.2"/>
@@ -8775,151 +8788,151 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="33" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="H2" s="36"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="37" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="39" t="s">
         <v>268</v>
       </c>
-      <c r="H3" s="38"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="39" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="H4" s="40"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="39" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="41" t="s">
         <v>272</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="41" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="43" t="s">
         <v>274</v>
       </c>
-      <c r="H6" s="42"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="39" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="45" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="B8" s="32" t="n">
+      <c r="B8" s="34" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="39" t="s">
+      <c r="C8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="45" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="35" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="37" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="39" t="s">
         <v>284</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -8927,13 +8940,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="44" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="46" t="s">
         <v>286</v>
       </c>
       <c r="H11" s="7" t="s">
@@ -8941,25 +8954,25 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="39" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="41" t="s">
         <v>288</v>
       </c>
       <c r="H12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="44" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="46" t="s">
         <v>289</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -8967,52 +8980,52 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="35" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37" t="s">
         <v>291</v>
       </c>
-      <c r="H14" s="36"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="37" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="39" t="s">
         <v>292</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="25" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="37" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="39" t="s">
         <v>294</v>
       </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="37" t="s">
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="39" t="s">
         <v>295</v>
       </c>
       <c r="H17" s="7" t="s">
@@ -9020,13 +9033,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="44" t="s">
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="46" t="s">
         <v>297</v>
       </c>
       <c r="H18" s="7" t="s">
@@ -9034,76 +9047,76 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="35" t="s">
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="H19" s="36"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="44" t="s">
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="46" t="s">
         <v>300</v>
       </c>
-      <c r="H20" s="38"/>
+      <c r="H20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="37" t="s">
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="39" t="s">
         <v>301</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="44" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="H22" s="38"/>
+      <c r="H22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="37" t="s">
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="39" t="s">
         <v>303</v>
       </c>
-      <c r="H23" s="38"/>
+      <c r="H23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="45" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="47" t="s">
         <v>304</v>
       </c>
-      <c r="H24" s="45"/>
+      <c r="H24" s="47"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10099,11 +10112,11 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.9"/>
@@ -10177,111 +10190,111 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
-        <v>1</v>
+      <c r="A5" s="15" t="s">
+        <v>308</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="E5" s="13" t="s">
         <v>310</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>311</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="15" t="n">
+      <c r="H5" s="16" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="J5" s="16"/>
+        <v>312</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="K5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
-        <v>2</v>
+      <c r="A6" s="15" t="s">
+        <v>313</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="C6" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>314</v>
+        <v>315</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="17" t="n">
+      <c r="H6" s="18" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="J6" s="18"/>
+        <v>312</v>
+      </c>
+      <c r="J6" s="19"/>
       <c r="K6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
-        <v>3</v>
+      <c r="A7" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="C7" s="46" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>242</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>317</v>
+        <v>319</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="47" t="n">
+      <c r="H7" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
+      <c r="I7" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
-        <v>4</v>
+      <c r="A8" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C8" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>203</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>320</v>
+        <v>323</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>324</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
-      <c r="H8" s="17" t="n">
+      <c r="H8" s="18" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="J8" s="18"/>
+        <v>312</v>
+      </c>
+      <c r="J8" s="19"/>
       <c r="K8" s="14"/>
     </row>
   </sheetData>

</xml_diff>